<commit_message>
niewe data ivm deadlines
</commit_message>
<xml_diff>
--- a/Deadlines.xlsx
+++ b/Deadlines.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas_2\Documents\Bachelorproef-Ansible-vs-Puppet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasdetemmerman/Documents/Bachelorproef-Ansible-vs-Puppet/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t xml:space="preserve">maandag </t>
   </si>
@@ -361,27 +367,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Deadline?   
+    <t>litteratuurstudie</t>
+  </si>
+  <si>
+    <t>Puppet manifest</t>
+  </si>
+  <si>
+    <t>Vagrant</t>
+  </si>
+  <si>
+    <t>Ansible playbook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final draft
 Einde stage             26      </t>
   </si>
   <si>
-    <t>litteratuurstudie</t>
-  </si>
-  <si>
-    <t>Puppet manifest</t>
-  </si>
-  <si>
-    <t>Vagrant</t>
-  </si>
-  <si>
-    <t>Ansible playbook</t>
+    <t>2
+Deadline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,8 +442,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +478,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -475,7 +498,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,7 +509,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,7 +537,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,7 +548,7 @@
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
     <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
     <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -530,6 +556,21 @@
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -558,21 +599,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -587,32 +613,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="K4:L15" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="K4:L15" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="K4:L15"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="onderdeel" dataDxfId="9"/>
-    <tableColumn id="2" name="sub-onderdeel" dataDxfId="8"/>
+    <tableColumn id="1" name="onderdeel" dataDxfId="5"/>
+    <tableColumn id="2" name="sub-onderdeel" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="M4:N15" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="M4:N15" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="M4:N15"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ref bp-voorstel" dataDxfId="6"/>
-    <tableColumn id="2" name="voltooid" dataCellStyle="Standaard"/>
+    <tableColumn id="1" name="ref bp-voorstel" dataDxfId="2"/>
+    <tableColumn id="2" name="voltooid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="J4:J16" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="J4:J16" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="J4:J16"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="N°" dataDxfId="1"/>
+    <tableColumn id="1" name="N°" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,27 +943,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="33" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="27.33203125" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>13</v>
       </c>
@@ -986,7 +1012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -1012,7 +1038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>27</v>
       </c>
@@ -1053,7 +1079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>6</v>
       </c>
@@ -1079,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
@@ -1089,7 +1115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>13</v>
       </c>
@@ -1125,7 +1151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>20</v>
       </c>
@@ -1152,14 +1178,14 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>27</v>
       </c>
@@ -1189,14 +1215,14 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1223,14 +1249,14 @@
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>10</v>
       </c>
@@ -1266,7 +1292,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>17</v>
       </c>
@@ -1302,7 +1328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>24</v>
       </c>
@@ -1341,7 +1367,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>1</v>
       </c>
@@ -1377,7 +1403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -1413,7 +1439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>15</v>
       </c>
@@ -1449,7 +1475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>22</v>
       </c>
@@ -1462,8 +1488,8 @@
       <c r="D16" s="8">
         <v>25</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>55</v>
+      <c r="E16" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="8">
         <v>27</v>
@@ -1483,7 +1509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>29</v>
       </c>
@@ -1496,8 +1522,8 @@
       <c r="D17" s="9">
         <v>1</v>
       </c>
-      <c r="E17" s="5">
-        <v>2</v>
+      <c r="E17" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F17" s="9">
         <v>3</v>
@@ -1512,7 +1538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -1537,13 +1563,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N5:N16">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="true">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH("true",N5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",N5)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>"false=$N$5"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
voltooide zaken groen gemarkeerd
</commit_message>
<xml_diff>
--- a/Deadlines.xlsx
+++ b/Deadlines.xlsx
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1275,7 @@
         <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="M7" s="3"/>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="M8" s="3"/>
       <c r="N8" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="M9" s="3"/>
       <c r="N9" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>